<commit_message>
columns to english done; before adding necessary options
</commit_message>
<xml_diff>
--- a/Liushui/output/sample3.xlsx
+++ b/Liushui/output/sample3.xlsx
@@ -437,67 +437,67 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>交易日期</t>
+          <t>date text</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>交易时间</t>
+          <t>time text</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>本方名称</t>
+          <t>sender_name text</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>本方账号</t>
+          <t>sender_account text</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>本方银行</t>
+          <t>sender_bank text</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>对方名称</t>
+          <t>receiver_name text</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>对方账号</t>
+          <t>receiver_account text</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>交易类型</t>
+          <t>type text</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>摘要</t>
+          <t>abstract text</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>流入金额</t>
+          <t>received_amount text</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>流出金额</t>
+          <t>sent_amount text</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>交易后余额</t>
+          <t>balance text</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>系统分类</t>
+          <t>system_classification text</t>
         </is>
       </c>
     </row>

</xml_diff>